<commit_message>
Fixing some missing geographic data in Angola context
</commit_message>
<xml_diff>
--- a/Data/Luanda/Misc/Adding_NOPerctangeChange.xlsx
+++ b/Data/Luanda/Misc/Adding_NOPerctangeChange.xlsx
@@ -28,10 +28,10 @@
     <t xml:space="preserve">NAME</t>
   </si>
   <si>
-    <t xml:space="preserve">Huambo City</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Luanda City</t>
+    <t xml:space="preserve">Huambo_City</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Luanda_City</t>
   </si>
   <si>
     <t xml:space="preserve">ZEE</t>
@@ -50,6 +50,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -71,6 +72,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -115,7 +117,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -125,6 +127,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -152,10 +158,10 @@
   <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+      <selection pane="topLeft" activeCell="I15" activeCellId="0" sqref="I15:J15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" s="1" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -187,89 +193,89 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2" s="3" t="n">
         <v>-0.107006863</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="C2" s="3" t="n">
         <v>-0.053411003</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="D2" s="3" t="n">
         <v>0.005631374</v>
       </c>
-      <c r="E2" s="0" t="n">
+      <c r="E2" s="3" t="n">
         <v>-0.020855071</v>
       </c>
-      <c r="F2" s="0" t="n">
+      <c r="F2" s="3" t="n">
         <v>-0.042518255</v>
       </c>
-      <c r="G2" s="0" t="n">
+      <c r="G2" s="3" t="n">
         <v>-0.042157895</v>
       </c>
-      <c r="H2" s="0" t="n">
+      <c r="H2" s="3" t="n">
         <v>0.02035211</v>
       </c>
-      <c r="I2" s="0" t="n">
+      <c r="I2" s="3" t="n">
         <v>0.059352687</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3" s="3" t="n">
         <v>-0.117256543</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="C3" s="3" t="n">
         <v>-0.23826728</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="D3" s="3" t="n">
         <v>-0.055835547</v>
       </c>
-      <c r="E3" s="0" t="n">
+      <c r="E3" s="3" t="n">
         <v>-0.009129526</v>
       </c>
-      <c r="F3" s="0" t="n">
+      <c r="F3" s="3" t="n">
         <v>0.030733355</v>
       </c>
-      <c r="G3" s="0" t="n">
+      <c r="G3" s="3" t="n">
         <v>-0.052397754</v>
       </c>
-      <c r="H3" s="0" t="n">
+      <c r="H3" s="3" t="n">
         <v>-0.006577813</v>
       </c>
-      <c r="I3" s="0" t="n">
+      <c r="I3" s="3" t="n">
         <v>-0.062237955</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4" s="3" t="n">
         <v>-0.148212391</v>
       </c>
-      <c r="C4" s="0" t="n">
+      <c r="C4" s="3" t="n">
         <v>-0.167682874</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="D4" s="3" t="n">
         <v>-0.059815112</v>
       </c>
-      <c r="E4" s="0" t="n">
+      <c r="E4" s="3" t="n">
         <v>0.116575327</v>
       </c>
-      <c r="F4" s="0" t="n">
+      <c r="F4" s="3" t="n">
         <v>0.006137356</v>
       </c>
-      <c r="G4" s="0" t="n">
+      <c r="G4" s="3" t="n">
         <v>-0.052624971</v>
       </c>
-      <c r="H4" s="0" t="n">
+      <c r="H4" s="3" t="n">
         <v>0.027426867</v>
       </c>
-      <c r="I4" s="0" t="n">
+      <c r="I4" s="3" t="n">
         <v>0.005947356</v>
       </c>
     </row>

</xml_diff>